<commit_message>
public code batch import python tools
</commit_message>
<xml_diff>
--- a/pub_code_batch_import/公共代码数据.xlsx
+++ b/pub_code_batch_import/公共代码数据.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\long\Desktop\工具类\公共代码批量导入\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\long\Desktop\local-python-tools\pub_code_batch_import\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B8EFC89-220F-4072-B5DC-595451DBADAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B59AFBA1-0033-449F-B7EC-CE834E5F8CEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="23520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="23520" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="变量" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="40">
   <si>
     <t>大类</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -54,18 +54,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>一般公共预算支出科目</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>一般公共预算收入科目</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>通用代码</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>一般公共服务支出</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -118,10 +106,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>读取sheet 类目，生成类目的insert语句</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>变量名</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -138,18 +122,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>creator</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>133229490020159488</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>modifier</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>tenant_id</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -163,6 +139,65 @@
   </si>
   <si>
     <t>175142360110354433</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>user_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SQL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select ds_hierarchy_id from ds_std_hierarchy where if_delete='0' and  cn_name = '公共代码' ;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select  ds_category_id from ds_std_category where if_delete='0' and  cn_name = '数据标准' and ds_hierarchy_id =  (select ds_hierarchy_id from ds_std_hierarchy where if_delete='0' and  cn_name = '公共代码') and parent_dgov_category_id = -1;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>一般公共预算支出科目1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>一般公共预算收入科目1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>通用代码1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>国内增值税</t>
+  </si>
+  <si>
+    <t>进口货物增值税</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>代码名称</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>标准编码</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>英文名称</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Domestic value-added tax</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Value added tax on imports</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>数据类型</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -170,7 +205,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -184,6 +219,13 @@
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF4D5F6E"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="3">
@@ -212,10 +254,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -496,10 +539,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -509,58 +552,53 @@
     <col min="3" max="3" width="32.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="2" t="s">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="B3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="2" t="s">
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>23</v>
       </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="B4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B5" s="2" t="s">
+      <c r="C5" t="s">
         <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -574,8 +612,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{623D0476-EBF4-409A-8EC6-76245255599C}">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N20" sqref="N20"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -598,84 +636,84 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
         <v>9</v>
-      </c>
-      <c r="C5" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -686,12 +724,76 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0438D613-0886-4486-8A1D-1A514F69F5FA}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="17.25" customWidth="1"/>
+    <col min="2" max="2" width="16.875" customWidth="1"/>
+    <col min="3" max="3" width="41.75" customWidth="1"/>
+    <col min="4" max="5" width="23.125" customWidth="1"/>
+    <col min="6" max="6" width="31.125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2">
+        <v>1010101</v>
+      </c>
+      <c r="E2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D3">
+        <v>1010102</v>
+      </c>
+      <c r="E3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>